<commit_message>
multiple arguments are done.
we can use multiple arguments for our API.
</commit_message>
<xml_diff>
--- a/test/DIAG/wifi.xlsx
+++ b/test/DIAG/wifi.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\code\lg\TIDL\Code_Generator\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="28800" windowHeight="12396" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="114">
   <si>
     <t>DID_WORK_FOR_DEFINE_0</t>
   </si>
@@ -212,6 +207,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Courier New"/>
+        <family val="3"/>
       </rPr>
       <t>Data</t>
     </r>
@@ -547,16 +543,19 @@
     <t>NULL</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>dataLen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -576,7 +575,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -584,21 +583,16 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
     </font>
     <font>
       <sz val="8"/>
@@ -615,7 +609,7 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -637,8 +631,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -656,35 +652,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -733,7 +731,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -783,7 +781,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -844,14 +842,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>640080</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>550551</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>108231</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>39651</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1203,26 +1201,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -1230,7 +1228,7 @@
       <c r="F1" s="2"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -1238,19 +1236,19 @@
       <c r="F2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8">
       <c r="A3" s="1"/>
       <c r="C3" s="1"/>
       <c r="F3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8">
       <c r="A4" s="1"/>
       <c r="C4" s="1"/>
       <c r="F4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1273,7 +1271,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1293,7 +1291,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1313,7 +1311,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1336,7 +1334,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1350,7 +1348,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1370,7 +1368,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1378,39 +1376,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6">
       <c r="A21" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1430,7 +1428,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
@@ -1450,7 +1448,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -1470,7 +1468,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
@@ -1490,7 +1488,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -1510,7 +1508,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1530,334 +1528,278 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G34" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
         <v>1</v>
       </c>
-      <c r="C35" t="s">
+      <c r="B49" t="s">
         <v>45</v>
       </c>
-      <c r="D35" t="s">
+      <c r="C49" t="s">
         <v>46</v>
       </c>
-      <c r="E35">
+      <c r="D49">
         <v>0</v>
       </c>
-      <c r="G35" t="s">
+      <c r="F49" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A36" s="1" t="s">
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50">
         <v>0</v>
       </c>
-      <c r="B36">
-        <v>2</v>
-      </c>
-      <c r="C36" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="F50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E51" t="s">
+        <v>113</v>
+      </c>
+      <c r="F51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" t="s">
+        <v>58</v>
+      </c>
+      <c r="D57" t="s">
+        <v>107</v>
+      </c>
+      <c r="E57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>104</v>
+      </c>
+      <c r="E58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>69</v>
+      </c>
+      <c r="B62" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="75">
+      <c r="A63" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="188">
+      <c r="A64" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>46</v>
+      </c>
+      <c r="B65" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>78</v>
+      </c>
+      <c r="B66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
         <v>49</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="G36" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="C37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" t="s">
-        <v>52</v>
-      </c>
-      <c r="E37" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" t="s">
-        <v>54</v>
-      </c>
-      <c r="G37" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>103</v>
-      </c>
-      <c r="D38" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A40" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A41" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A42" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A44" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A45" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A50" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A51">
-        <v>1</v>
-      </c>
-      <c r="B51" t="s">
-        <v>45</v>
-      </c>
-      <c r="C51" t="s">
-        <v>46</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="F51" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A52">
-        <v>2</v>
-      </c>
-      <c r="B52" t="s">
-        <v>48</v>
-      </c>
-      <c r="C52" t="s">
-        <v>49</v>
-      </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="F52" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A53">
-        <v>3</v>
-      </c>
-      <c r="B53" t="s">
-        <v>51</v>
-      </c>
-      <c r="C53" t="s">
-        <v>52</v>
-      </c>
-      <c r="D53" t="s">
-        <v>53</v>
-      </c>
-      <c r="E53" t="s">
-        <v>54</v>
-      </c>
-      <c r="F53" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A59" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B59" t="s">
-        <v>57</v>
-      </c>
-      <c r="C59" t="s">
-        <v>58</v>
-      </c>
-      <c r="D59" t="s">
-        <v>107</v>
-      </c>
-      <c r="E59" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>104</v>
-      </c>
-      <c r="E60" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
-        <v>63</v>
-      </c>
-      <c r="B62" t="s">
-        <v>64</v>
-      </c>
-      <c r="C62" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
-        <v>66</v>
-      </c>
-      <c r="B63" t="s">
-        <v>67</v>
-      </c>
-      <c r="C63" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
-        <v>69</v>
-      </c>
-      <c r="B64" t="s">
-        <v>70</v>
-      </c>
-      <c r="C64" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="96" x14ac:dyDescent="0.45">
-      <c r="A65" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="175.2" x14ac:dyDescent="0.45">
-      <c r="A66" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
-        <v>46</v>
       </c>
       <c r="B67" t="s">
         <v>70</v>
@@ -1866,9 +1808,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B68" t="s">
         <v>70</v>
@@ -1877,74 +1819,52 @@
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B69" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C69" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C70" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B71" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C71" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
-        <v>82</v>
-      </c>
-      <c r="B72" t="s">
-        <v>83</v>
-      </c>
-      <c r="C72" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
-        <v>84</v>
-      </c>
-      <c r="B73" t="s">
-        <v>85</v>
-      </c>
-      <c r="C73" t="s">
         <v>86</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C51:C54 D35:D37">
-      <formula1>$A$61:$A$73</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C49:C52 D35">
+      <formula1>$A$59:$A$71</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D38 C19:C20 G39:G46 C39:C46 G19:G20 D8:D18">
-      <formula1>$A$60:$A$73</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D36 D8:D18 G19:G20 C37:C44 G37:G44 C19:C20">
+      <formula1>$A$58:$A$71</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>